<commit_message>
added Frank to the list of speakers
</commit_message>
<xml_diff>
--- a/docs/Affiliation_and_website.xlsx
+++ b/docs/Affiliation_and_website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/Ocean_Data_Bootcamp/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D120DA-712E-2D43-A0CE-232A1C28BA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E0C7DE-661A-8F48-8941-AD2803DBF6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="1840" windowWidth="35840" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1840" windowWidth="35840" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>https://peldhces.wordpress.com/</t>
+  </si>
+  <si>
+    <t>Frank Muller-Karger</t>
+  </si>
+  <si>
+    <t>U. South Florida / MBON</t>
+  </si>
+  <si>
+    <t>https://www.usf.edu/marine-science/faculty/faculty-directory/biological-oceanography/frank-muller-karger.aspx</t>
+  </si>
+  <si>
+    <t>carib@usf.edu</t>
   </si>
 </sst>
 </file>
@@ -402,10 +414,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -543,55 +555,70 @@
     </row>
     <row r="10" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C8:C9" r:id="rId2" display="https://www.aoml.noaa.gov/ocean-chemistry-ecosystems-division/" xr:uid="{4590DE3C-707B-C145-A097-38CE82FAB499}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to agenda, participants, and speakers pages
</commit_message>
<xml_diff>
--- a/docs/Affiliation_and_website.xlsx
+++ b/docs/Affiliation_and_website.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enriquemontes/Ocean_Data_Bootcamp/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E0C7DE-661A-8F48-8941-AD2803DBF6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEDCD6-5DC6-DB41-B0B6-EE48D8A3B767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1840" windowWidth="35840" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="720" windowWidth="35840" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -37,12 +37,6 @@
     <t>https://www.aoml.noaa.gov/ocean-chemistry-ecosystems-division/</t>
   </si>
   <si>
-    <t>enrique.montes@noaa.gov</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Cesar Cordeiro</t>
   </si>
   <si>
@@ -100,27 +94,12 @@
     <t>Bioenv Análises Ambientais</t>
   </si>
   <si>
-    <t>cesarcordeiro@uenf.br</t>
-  </si>
-  <si>
     <t>https://peldiloc.sites.ufsc.br/boia-oceanografica-peld-iloc-no-arquipelago-fernando-de-noronha/</t>
   </si>
   <si>
     <t>https://benderlab.weebly.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">kelly.montenero@noaa.gov </t>
-  </si>
-  <si>
-    <t xml:space="preserve">willem.klajbor@noaa.gov </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ac.mazzuco@me.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">angelofraga@gmail.com </t>
-  </si>
-  <si>
     <t>https://www.iatlantic.eu/our-team/iatlantic-fellows/</t>
   </si>
   <si>
@@ -145,14 +124,71 @@
     <t>https://www.usf.edu/marine-science/faculty/faculty-directory/biological-oceanography/frank-muller-karger.aspx</t>
   </si>
   <si>
-    <t>carib@usf.edu</t>
+    <t>Alexandre Braga</t>
+  </si>
+  <si>
+    <t>Oceano Digital</t>
+  </si>
+  <si>
+    <t>https://www.oceanodigital.com.br/ </t>
+  </si>
+  <si>
+    <t>Barbara Ramos Pinheiro</t>
+  </si>
+  <si>
+    <t>PELD Costa dos Corais</t>
+  </si>
+  <si>
+    <t>https://icbs.ufal.br/pt-br/pos-graduacao/diversidade-biologica-e-conservacao-nos-tropicos/institucional/peld-apacc-al</t>
+  </si>
+  <si>
+    <t>Jonathas Barreto</t>
+  </si>
+  <si>
+    <t>Laboratório de Nectologia da UFES</t>
+  </si>
+  <si>
+    <t>Felipe Azevedo Bastos</t>
+  </si>
+  <si>
+    <t>IEMA</t>
+  </si>
+  <si>
+    <r>
+      <t>https://www.linkedin.com/in/jonathas-barreto-b56492120/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>https://iema.es.gov.br/gerenciamento-costeiro</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,9 +201,42 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -192,10 +261,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +487,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -428,198 +501,226 @@
     <col min="4" max="4" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C8:C9" r:id="rId2" display="https://www.aoml.noaa.gov/ocean-chemistry-ecosystems-division/" xr:uid="{4590DE3C-707B-C145-A097-38CE82FAB499}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{8DFA410D-22C5-D749-A0E1-DBB127DE850A}"/>
+    <hyperlink ref="C13" r:id="rId4" display="https://www.linkedin.com/in/jonathas-barreto-b56492120/" xr:uid="{C97CBD5E-DAC3-354B-8E05-771A6E414624}"/>
+    <hyperlink ref="C14" r:id="rId5" display="https://iema.es.gov.br/gerenciamento-costeiro" xr:uid="{84CCBD11-1A5D-A046-BADF-2FEC7365DE45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>